<commit_message>
Added checks for required fields in Edit Asset.
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784EAB85-1DF7-4416-8332-46CE3E19F68E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0575E85F-2A53-44C4-A5F8-6FDF4237B614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="1260" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -449,13 +449,40 @@
   </si>
   <si>
     <t>マシン処理済。マシン名：{0} / Id：{1}。</t>
+  </si>
+  <si>
+    <t>ProcessedEditUser</t>
+  </si>
+  <si>
+    <t>ユーザー処理済。 Id：{0}。</t>
+  </si>
+  <si>
+    <t>User already processed. Id: {0}.</t>
+  </si>
+  <si>
+    <t>UserIdNotSpecified</t>
+  </si>
+  <si>
+    <t>Id not specified for user named: {0}.</t>
+  </si>
+  <si>
+    <t>{0}というユーザーのIDが指定されませんでした。</t>
+  </si>
+  <si>
+    <t>AssetNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Name not specified for asset with Id: {0}.</t>
+  </si>
+  <si>
+    <t>ID{0}アセットの名前が指定されませんでした。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,16 +498,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -488,19 +528,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -537,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C41" totalsRowShown="0">
-  <autoFilter ref="A1:C41" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C43" totalsRowShown="0">
+  <autoFilter ref="A1:C43" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -813,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -969,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,309 +1174,340 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>147</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>103</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>144</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Made it possible to delete robot by passing Robot Name, in addition to Robot Id.
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73F65F5-A836-4E8C-B092-6021E807626D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD52375-C483-4DB3-8EEE-60B44ACFBC80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="181">
   <si>
     <t>Name</t>
   </si>
@@ -223,18 +223,12 @@
     <t>選択された操作が多数のAPIリクエストを行う予想します。よろしいですか。</t>
   </si>
   <si>
-    <t>Failed to get folders. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
     <t>フォルダ取得が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
   </si>
   <si>
     <t>GetMachinesFailure</t>
   </si>
   <si>
-    <t>GetFoldersFailure</t>
-  </si>
-  <si>
     <t>OrchestratorVersion</t>
   </si>
   <si>
@@ -247,12 +241,6 @@
     <t>ユーザーが多数のAPIリクエストを行うこと承認しました。</t>
   </si>
   <si>
-    <t>ChooseFolderMessage</t>
-  </si>
-  <si>
-    <t>ChooseFolderTitle</t>
-  </si>
-  <si>
     <t>組織単位（フォルダ）</t>
   </si>
   <si>
@@ -382,9 +370,6 @@
     <t>ユーザー取得が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
   </si>
   <si>
-    <t>GetFolderFailure</t>
-  </si>
-  <si>
     <t>Failed to get organization unit (folder) with Id: {0}. Request status: {1} / Response: {2}.</t>
   </si>
   <si>
@@ -529,9 +514,6 @@
     <t>DeleteRobotResultColumn</t>
   </si>
   <si>
-    <t>FolderNotFound</t>
-  </si>
-  <si>
     <t>The Organization Unit (Folder) named {0} was not found.</t>
   </si>
   <si>
@@ -560,6 +542,33 @@
   </si>
   <si>
     <t>{0}というマシンが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>RobotNotFound</t>
+  </si>
+  <si>
+    <t>The robot named {0} was not found.</t>
+  </si>
+  <si>
+    <t>{0}というロボットが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>Failed to get OUs. Request status: {0} / Response: {1}.</t>
+  </si>
+  <si>
+    <t>ChooseOUMessage</t>
+  </si>
+  <si>
+    <t>ChooseOUTitle</t>
+  </si>
+  <si>
+    <t>GetOUFailure</t>
+  </si>
+  <si>
+    <t>OUNotFound</t>
+  </si>
+  <si>
+    <t>GetOUsFailure</t>
   </si>
 </sst>
 </file>
@@ -924,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -948,15 +957,15 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>201804</v>
@@ -1012,7 +1021,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
@@ -1020,23 +1029,23 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
@@ -1044,23 +1053,23 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s">
         <v>46</v>
@@ -1068,15 +1077,15 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
@@ -1084,18 +1093,18 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1114,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,46 +1246,46 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,10 +1293,10 @@
         <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1336,7 +1345,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>49</v>
@@ -1347,35 +1356,35 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1413,271 +1422,278 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>180</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="A51" t="s">
+        <v>172</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>

</xml_diff>

<commit_message>
Refactor files related to Machines
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC61ED3-B180-4467-BE9F-00D0D896300C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935069F8-BB50-4A55-9A72-3BDABB1C3C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="170">
   <si>
     <t>Name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Explanation</t>
   </si>
   <si>
-    <t>ProcessedMachine</t>
-  </si>
-  <si>
     <t>UnsupportedOperation</t>
   </si>
   <si>
@@ -150,18 +147,12 @@
     <t>選択されたエンティティが対応できません。</t>
   </si>
   <si>
-    <t>CreateMachineFailure</t>
-  </si>
-  <si>
     <t>CreateMachineResultColumn</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>DeleteMachineFailure</t>
-  </si>
-  <si>
     <t>OperationDefaultResult</t>
   </si>
   <si>
@@ -177,24 +168,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Failed to create machine. Type: {0} / Name: {1}. Request status: {2} / Response: {3}.</t>
-  </si>
-  <si>
-    <t>Failed to delete machine. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>Failed to get machines. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>マシン削除が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
-  </si>
-  <si>
-    <t>マシン作成が失敗しました。タイプ：{0} / 名前：{1}。リクエストステータス： {2} / レスポンス：{3}。</t>
-  </si>
-  <si>
-    <t>マシン取得が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
-  </si>
-  <si>
     <t>MachineConfigFilepath</t>
   </si>
   <si>
@@ -225,9 +198,6 @@
     <t>選択された操作が多数のAPIリクエストを行う予想します。よろしいですか。</t>
   </si>
   <si>
-    <t>GetMachinesFailure</t>
-  </si>
-  <si>
     <t>OrchestratorVersion</t>
   </si>
   <si>
@@ -294,24 +264,6 @@
     <t>https://platform.uipath.com/OrganizationName/ServiceName</t>
   </si>
   <si>
-    <t>GetUsersFailure</t>
-  </si>
-  <si>
-    <t>Failed to get users. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>ユーザー取得が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
-  </si>
-  <si>
-    <t>CreateUserFailure</t>
-  </si>
-  <si>
-    <t>Failed to create user. UserName: {0}. Request status: {1} / Response: {2}.</t>
-  </si>
-  <si>
-    <t>ユーザー作成が失敗しました。ユーザー名：{0}。リクエストステータス： {1} / レスポンス：{2}。</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -324,39 +276,18 @@
     <t>ProcessedUser</t>
   </si>
   <si>
-    <t>DeleteUserFailure</t>
-  </si>
-  <si>
-    <t>Failed to delete user. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>ユーザー削除が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
-  </si>
-  <si>
     <t>DeleteUserResultColumn</t>
   </si>
   <si>
     <t>User already processed. UserName: {0} / Id: {1}.</t>
   </si>
   <si>
-    <t>Machine already processed. Machine name: {0} / Id: {1}.</t>
-  </si>
-  <si>
     <t>ProcessedEditUser</t>
   </si>
   <si>
     <t>User already processed. Id: {0}.</t>
   </si>
   <si>
-    <t>EditUserFailure</t>
-  </si>
-  <si>
-    <t>Failed to edit user: Id: {0}. Request status: {1} / Response: {2}.</t>
-  </si>
-  <si>
-    <t>ユーザー編集が失敗しました。ID：{0}。リクエストステータス：{1} / レスポンス：{2}。</t>
-  </si>
-  <si>
     <t>EditUserResultColumn</t>
   </si>
   <si>
@@ -369,15 +300,6 @@
     <t>Config\JA\ロボット.xlsx</t>
   </si>
   <si>
-    <t>GetRobotsFailure</t>
-  </si>
-  <si>
-    <t>Failed to get robots. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>ロボット取得が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
-  </si>
-  <si>
     <t>ProcessedRobot</t>
   </si>
   <si>
@@ -393,30 +315,9 @@
     <t>ロボット処理済。ロボット名：{0} / ID：{1}。</t>
   </si>
   <si>
-    <t>マシン処理済。マシン名：{0} / ID：{1}。</t>
-  </si>
-  <si>
-    <t>DeleteRobotFailure</t>
-  </si>
-  <si>
-    <t>Failed to delete robot. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>ロボット削除が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
-  </si>
-  <si>
     <t>DeleteRobotResultColumn</t>
   </si>
   <si>
-    <t>CreateRobotFailure</t>
-  </si>
-  <si>
-    <t>Failed to create robot. Name: {0}. Request status: {1} / Response: {2}.</t>
-  </si>
-  <si>
-    <t>ロボット作成が失敗しました。名前：{0}。リクエストステータス： {1} / レスポンス：{2}。</t>
-  </si>
-  <si>
     <t>CreateRobotResultColumn</t>
   </si>
   <si>
@@ -447,9 +348,6 @@
     <t>CreateRobottIDColumn</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>CreateMachineIDColumn</t>
   </si>
   <si>
@@ -507,9 +405,6 @@
     <t>組織単位が見つかりませんでした。</t>
   </si>
   <si>
-    <t>No Machine found.</t>
-  </si>
-  <si>
     <t>ロボットが見つかりませんでした。</t>
   </si>
   <si>
@@ -525,9 +420,6 @@
     <t>No Environment found.</t>
   </si>
   <si>
-    <t>No Robot found.</t>
-  </si>
-  <si>
     <t>Type not specified.</t>
   </si>
   <si>
@@ -619,6 +511,39 @@
   </si>
   <si>
     <t>The specified Asset ID and Asset name do not match.</t>
+  </si>
+  <si>
+    <t>IDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>NameNotSpecified</t>
+  </si>
+  <si>
+    <t>IDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>ID invalid or not specified.</t>
+  </si>
+  <si>
+    <t>Name not specified.</t>
+  </si>
+  <si>
+    <t>The specified ID and Name do not match.</t>
+  </si>
+  <si>
+    <t>IDが無効か指定されませんでした。</t>
+  </si>
+  <si>
+    <t>名前が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>指定された名前とIDが一致しません。</t>
+  </si>
+  <si>
+    <t>Machine not found.</t>
+  </si>
+  <si>
+    <t>Robot not found.</t>
   </si>
 </sst>
 </file>
@@ -707,8 +632,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C68" totalsRowShown="0">
-  <autoFilter ref="A1:C68" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C60" totalsRowShown="0">
+  <autoFilter ref="A1:C60" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -984,7 +909,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,15 +932,15 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>201804</v>
@@ -1039,122 +964,122 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1171,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1197,46 +1122,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1339,474 +1264,386 @@
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="A26" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>75</v>
+        <v>163</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>165</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>166</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>178</v>
+        <v>65</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>179</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>183</v>
+        <v>120</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>185</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>189</v>
+        <v>129</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>194</v>
+        <v>128</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="A33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>158</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>104</v>
+      <c r="A38" t="s">
+        <v>82</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>102</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>113</v>
-      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>58</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>125</v>
+        <v>59</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>129</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>158</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>70</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>134</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>180</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>186</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>191</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>150</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>142</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor files related to Users
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935069F8-BB50-4A55-9A72-3BDABB1C3C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2262FC56-9C9B-4FF5-8358-03B0F7504A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="176">
   <si>
     <t>Name</t>
   </si>
@@ -273,21 +273,9 @@
     <t>I</t>
   </si>
   <si>
-    <t>ProcessedUser</t>
-  </si>
-  <si>
     <t>DeleteUserResultColumn</t>
   </si>
   <si>
-    <t>User already processed. UserName: {0} / Id: {1}.</t>
-  </si>
-  <si>
-    <t>ProcessedEditUser</t>
-  </si>
-  <si>
-    <t>User already processed. Id: {0}.</t>
-  </si>
-  <si>
     <t>EditUserResultColumn</t>
   </si>
   <si>
@@ -306,12 +294,6 @@
     <t>Robot already processed. Robot name: {0} / Id: {1}.</t>
   </si>
   <si>
-    <t>ユーザー処理済。ユーザー名：{0} / ID：{1}。</t>
-  </si>
-  <si>
-    <t>ユーザー処理済。 ID：{0}。</t>
-  </si>
-  <si>
     <t>ロボット処理済。ロボット名：{0} / ID：{1}。</t>
   </si>
   <si>
@@ -544,6 +526,42 @@
   </si>
   <si>
     <t>Robot not found.</t>
+  </si>
+  <si>
+    <t>UserNotFound</t>
+  </si>
+  <si>
+    <t>User not  found.</t>
+  </si>
+  <si>
+    <t>ユーザーが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>StatusNotSupported</t>
+  </si>
+  <si>
+    <t>Status not supported.</t>
+  </si>
+  <si>
+    <t>指定されたステータスが対応できません。</t>
+  </si>
+  <si>
+    <t>UsernameNotSpecified</t>
+  </si>
+  <si>
+    <t>Username not specified.</t>
+  </si>
+  <si>
+    <t>ユーザー名が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>IDAndUsernameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified ID and Username do not match.</t>
+  </si>
+  <si>
+    <t>指定されたIDとユーザー名が一致しません。</t>
   </si>
 </sst>
 </file>
@@ -632,8 +650,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C60" totalsRowShown="0">
-  <autoFilter ref="A1:C60" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C62" totalsRowShown="0">
+  <autoFilter ref="A1:C62" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -909,7 +927,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -980,7 +998,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
@@ -988,7 +1006,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
@@ -996,7 +1014,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
         <v>68</v>
@@ -1007,7 +1025,7 @@
         <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1015,7 +1033,7 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1028,7 +1046,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
         <v>76</v>
@@ -1044,7 +1062,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
         <v>43</v>
@@ -1052,7 +1070,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
         <v>78</v>
@@ -1060,7 +1078,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
@@ -1068,7 +1086,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
         <v>76</v>
@@ -1076,7 +1094,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
         <v>78</v>
@@ -1096,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1144,13 +1162,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1313,13 +1331,13 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1335,79 +1353,79 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1427,57 +1445,57 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1486,164 +1504,186 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>60</v>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>102</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>156</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>125</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standardize workflows that create entities
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D2E1CC-C533-4CDD-A08E-269577AA9F2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E265147-6E8F-403F-A4AD-B3A2497325D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="217">
   <si>
     <t>Name</t>
   </si>
@@ -345,9 +345,6 @@
     <t>CreateUserIDColumn</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
     <t>AssetNotFound</t>
   </si>
   <si>
@@ -670,6 +667,24 @@
   </si>
   <si>
     <t>Add Or Remove Robots</t>
+  </si>
+  <si>
+    <t>SurnameNotSpecified</t>
+  </si>
+  <si>
+    <t>Surname not specified.</t>
+  </si>
+  <si>
+    <t>性が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>EmailNotSpecified</t>
+  </si>
+  <si>
+    <t>Email not specified.</t>
+  </si>
+  <si>
+    <t>メールアドレスが指定されませんでした。</t>
   </si>
 </sst>
 </file>
@@ -758,8 +773,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C69" totalsRowShown="0">
-  <autoFilter ref="A1:C69" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C71" totalsRowShown="0">
+  <autoFilter ref="A1:C71" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1034,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,7 +1140,7 @@
         <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1133,7 +1148,7 @@
         <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1205,12 +1220,12 @@
         <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B21" t="s">
         <v>76</v>
@@ -1218,7 +1233,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
@@ -1226,7 +1241,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
@@ -1234,7 +1249,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B24" t="s">
         <v>38</v>
@@ -1242,7 +1257,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B25" t="s">
         <v>38</v>
@@ -1262,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1332,13 +1347,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1391,13 +1406,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1505,13 +1520,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1549,127 +1564,127 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1678,274 +1693,296 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="A44" t="s">
+        <v>211</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>214</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>85</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>171</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="A53" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>207</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>151</v>
+        <v>208</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>108</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>88</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>174</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>171</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>127</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>179</v>
-      </c>
-      <c r="B64" t="s">
-        <v>180</v>
-      </c>
-      <c r="C64" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>194</v>
-      </c>
-      <c r="B65" t="s">
-        <v>195</v>
-      </c>
-      <c r="C65" t="s">
-        <v>196</v>
+        <v>96</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>197</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>198</v>
+        <v>178</v>
+      </c>
+      <c r="B66" t="s">
+        <v>179</v>
       </c>
       <c r="C66" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>200</v>
+      </c>
+      <c r="B69" t="s">
         <v>201</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C69" t="s">
         <v>202</v>
-      </c>
-      <c r="C67" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Present forms for authentication and choosing of entity and operation
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E265147-6E8F-403F-A4AD-B3A2497325D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3990E970-969C-4319-BB0C-71C1511B84B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="255">
   <si>
     <t>Name</t>
   </si>
@@ -261,9 +261,6 @@
     <t>OrchestratorURL</t>
   </si>
   <si>
-    <t>https://platform.uipath.com/OrganizationName/ServiceName</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -685,6 +682,123 @@
   </si>
   <si>
     <t>メールアドレスが指定されませんでした。</t>
+  </si>
+  <si>
+    <t>Orchestrator Manager</t>
+  </si>
+  <si>
+    <t>FormTitle</t>
+  </si>
+  <si>
+    <t>ControlPanelTemplatePath</t>
+  </si>
+  <si>
+    <t>ControlPanelPath</t>
+  </si>
+  <si>
+    <t>FormPasswordLabel</t>
+  </si>
+  <si>
+    <t>FormUsernameLabel</t>
+  </si>
+  <si>
+    <t>FormEntityLabel</t>
+  </si>
+  <si>
+    <t>FormOperationLabel</t>
+  </si>
+  <si>
+    <t>FormSubmitButton</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ユーザー名</t>
+  </si>
+  <si>
+    <t>パスワード</t>
+  </si>
+  <si>
+    <t>送信</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>アセット</t>
+  </si>
+  <si>
+    <t>ユーザー</t>
+  </si>
+  <si>
+    <t>マシン</t>
+  </si>
+  <si>
+    <t>ロボット</t>
+  </si>
+  <si>
+    <t>ロボットグループ</t>
+  </si>
+  <si>
+    <t>FormAssetOption</t>
+  </si>
+  <si>
+    <t>FormUserOption</t>
+  </si>
+  <si>
+    <t>FormMachineOption</t>
+  </si>
+  <si>
+    <t>FormRobotOption</t>
+  </si>
+  <si>
+    <t>FormEnvironmentOption</t>
+  </si>
+  <si>
+    <t>AuthenticationPanelTemplatePath</t>
+  </si>
+  <si>
+    <t>Forms\ControlPanel.html</t>
+  </si>
+  <si>
+    <t>Forms\ControlPanelTemplate.html</t>
+  </si>
+  <si>
+    <t>Forms\AuthenticationPanelTemplate.html</t>
+  </si>
+  <si>
+    <t>AuthenticationPanelPath</t>
+  </si>
+  <si>
+    <t>Forms\AuthenticationPanel.html</t>
+  </si>
+  <si>
+    <t>OrchestratorTenant</t>
+  </si>
+  <si>
+    <t>MateusTenant</t>
+  </si>
+  <si>
+    <t>https://platform.uipath.com</t>
   </si>
 </sst>
 </file>
@@ -761,8 +875,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C25" totalsRowShown="0">
-  <autoFilter ref="A1:C25" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C30" totalsRowShown="0">
+  <autoFilter ref="A1:C30" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -773,8 +887,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C71" totalsRowShown="0">
-  <autoFilter ref="A1:C71" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C83" totalsRowShown="0">
+  <autoFilter ref="A1:C83" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1047,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,132 +1190,132 @@
         <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3">
-        <v>201804</v>
+        <v>252</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>201804</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>219</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>246</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
@@ -1209,63 +1323,103 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>199</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>203</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>198</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>187</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>202</v>
+      </c>
+      <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{A57A0458-685C-47C8-9CD5-9DD59357B9F2}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{88652A11-02F0-4DF5-B001-517D63DD6C16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1277,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1303,116 +1457,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>217</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>221</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>225</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>227</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>222</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>223</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>192</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>241</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>235</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>242</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>234</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>233</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>244</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>232</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>245</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1421,477 +1582,481 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>203</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>209</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>144</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>147</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>142</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>145</v>
+        <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>148</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>149</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A39" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>211</v>
+        <v>110</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>212</v>
+        <v>109</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>214</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="A46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>206</v>
+        <v>112</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>174</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>176</v>
-      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="A55" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>150</v>
+        <v>211</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>107</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>213</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>59</v>
+        <v>214</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>60</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>171</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>173</v>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>105</v>
@@ -1899,90 +2064,204 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>138</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>96</v>
+        <v>183</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>108</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>178</v>
-      </c>
-      <c r="B66" t="s">
-        <v>179</v>
-      </c>
-      <c r="C66" t="s">
-        <v>180</v>
+        <v>206</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>193</v>
-      </c>
-      <c r="B67" t="s">
-        <v>194</v>
-      </c>
-      <c r="C67" t="s">
-        <v>195</v>
-      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>196</v>
+        <v>87</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C68" t="s">
-        <v>198</v>
+        <v>149</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>170</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>131</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>136</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>177</v>
+      </c>
+      <c r="B78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>192</v>
+      </c>
+      <c r="B79" t="s">
+        <v>193</v>
+      </c>
+      <c r="C79" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>195</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C80" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>199</v>
+      </c>
+      <c r="B81" t="s">
         <v>200</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C81" t="s">
         <v>201</v>
-      </c>
-      <c r="C69" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Repeatedly prompt user for authentication and operation until the execution is stopped
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3990E970-969C-4319-BB0C-71C1511B84B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A1FA9A-670A-4742-821E-7D8340D4CEE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="261">
   <si>
     <t>Name</t>
   </si>
@@ -799,6 +799,24 @@
   </si>
   <si>
     <t>https://platform.uipath.com</t>
+  </si>
+  <si>
+    <t>FormCancelButton</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>キャンセル</t>
+  </si>
+  <si>
+    <t>The execution has been stopped.</t>
+  </si>
+  <si>
+    <t>StoppedExecution</t>
+  </si>
+  <si>
+    <t>実行が停止されました。</t>
   </si>
 </sst>
 </file>
@@ -887,8 +905,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C83" totalsRowShown="0">
-  <autoFilter ref="A1:C83" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C85" totalsRowShown="0">
+  <autoFilter ref="A1:C85" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1431,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1512,755 +1530,777 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>189</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>203</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>259</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>258</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>102</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="A51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>154</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>156</v>
-      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>210</v>
+        <v>157</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>211</v>
+        <v>158</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>212</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>213</v>
+        <v>160</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>214</v>
+        <v>161</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>215</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="A58" t="s">
+        <v>210</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>213</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>84</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>88</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>83</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>165</v>
+        <v>205</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="A67" t="s">
+        <v>183</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>87</v>
+        <v>206</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>106</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>58</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>87</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>172</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>58</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>170</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>103</v>
+        <v>171</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>125</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>131</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>177</v>
-      </c>
-      <c r="B78" t="s">
-        <v>178</v>
-      </c>
-      <c r="C78" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>192</v>
-      </c>
-      <c r="B79" t="s">
-        <v>193</v>
-      </c>
-      <c r="C79" t="s">
-        <v>194</v>
+        <v>95</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>195</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>196</v>
+        <v>177</v>
+      </c>
+      <c r="B80" t="s">
+        <v>178</v>
       </c>
       <c r="C80" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>192</v>
+      </c>
+      <c r="B81" t="s">
+        <v>193</v>
+      </c>
+      <c r="C81" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>195</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>199</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B83" t="s">
         <v>200</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adapt to work with Orchestrator 2018.4
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A1FA9A-670A-4742-821E-7D8340D4CEE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D00DB5-ABC0-40FD-9411-3C92BD5A9141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="266">
   <si>
     <t>Name</t>
   </si>
@@ -198,9 +198,6 @@
     <t>選択された操作が多数のAPIリクエストを行う予想します。よろしいですか。</t>
   </si>
   <si>
-    <t>OrchestratorVersion</t>
-  </si>
-  <si>
     <t>NumerousRequestsConfirmed</t>
   </si>
   <si>
@@ -525,9 +522,6 @@
     <t>指定されたIDとユーザー名が一致しません。</t>
   </si>
   <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>HostingTypeNotSpecified</t>
   </si>
   <si>
@@ -777,46 +771,67 @@
     <t>AuthenticationPanelTemplatePath</t>
   </si>
   <si>
-    <t>Forms\ControlPanel.html</t>
-  </si>
-  <si>
-    <t>Forms\ControlPanelTemplate.html</t>
-  </si>
-  <si>
-    <t>Forms\AuthenticationPanelTemplate.html</t>
-  </si>
-  <si>
     <t>AuthenticationPanelPath</t>
   </si>
   <si>
-    <t>Forms\AuthenticationPanel.html</t>
-  </si>
-  <si>
     <t>OrchestratorTenant</t>
   </si>
   <si>
+    <t>FormCancelButton</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>キャンセル</t>
+  </si>
+  <si>
+    <t>The execution has been stopped.</t>
+  </si>
+  <si>
+    <t>StoppedExecution</t>
+  </si>
+  <si>
+    <t>実行が停止されました。</t>
+  </si>
+  <si>
+    <t>FormAccountLockoutWarning</t>
+  </si>
+  <si>
+    <t>Please mind that many unncessful login attempts can temporarily lock the account, as specified in the Security settings of the tenant.</t>
+  </si>
+  <si>
+    <t>テナントの設定により、ログイン試行に複数回失敗した場合、アカウントを指定された秒数の間ロックされることご注意ください。</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>RobotAddedAndRemoved</t>
+  </si>
+  <si>
+    <t>ロボットが同時に追加・削除されています。</t>
+  </si>
+  <si>
+    <t>A robot is being added and removed at the same time.</t>
+  </si>
+  <si>
+    <t>https://platform.uipath.com</t>
+  </si>
+  <si>
     <t>MateusTenant</t>
   </si>
   <si>
-    <t>https://platform.uipath.com</t>
-  </si>
-  <si>
-    <t>FormCancelButton</t>
-  </si>
-  <si>
-    <t>Cancel</t>
-  </si>
-  <si>
-    <t>キャンセル</t>
-  </si>
-  <si>
-    <t>The execution has been stopped.</t>
-  </si>
-  <si>
-    <t>StoppedExecution</t>
-  </si>
-  <si>
-    <t>実行が停止されました。</t>
+    <t>Misc\Forms\ControlPanelTemplate.html</t>
+  </si>
+  <si>
+    <t>Misc\Forms\ControlPanel.html</t>
+  </si>
+  <si>
+    <t>Misc\Forms\AuthenticationPanelTemplate.html</t>
+  </si>
+  <si>
+    <t>Misc\Forms\AuthenticationPanel.html</t>
   </si>
 </sst>
 </file>
@@ -893,8 +908,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C30" totalsRowShown="0">
-  <autoFilter ref="A1:C30" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C29" totalsRowShown="0">
+  <autoFilter ref="A1:C29" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -905,8 +920,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C85" totalsRowShown="0">
-  <autoFilter ref="A1:C85" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C87" totalsRowShown="0">
+  <autoFilter ref="A1:C87" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1179,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1205,90 +1220,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B4">
-        <v>201804</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>216</v>
+      </c>
+      <c r="B6" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>251</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1296,31 +1311,31 @@
         <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
         <v>67</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1328,31 +1343,31 @@
         <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1360,98 +1375,87 @@
         <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>184</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>202</v>
-      </c>
-      <c r="B30" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{88652A11-02F0-4DF5-B001-517D63DD6C16}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1475,833 +1479,855 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>228</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>225</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>235</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>236</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>256</v>
+        <v>224</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>203</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>209</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>204</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>259</v>
+        <v>201</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>258</v>
+        <v>207</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>260</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="A27" t="s">
+        <v>251</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>151</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>210</v>
+        <v>159</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>208</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>211</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>83</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>150</v>
+        <v>203</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>181</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>204</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>87</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>58</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>172</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>103</v>
+        <v>169</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>125</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>130</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>176</v>
+        <v>137</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>177</v>
-      </c>
-      <c r="B80" t="s">
-        <v>178</v>
-      </c>
-      <c r="C80" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>192</v>
-      </c>
-      <c r="B81" t="s">
-        <v>193</v>
-      </c>
-      <c r="C81" t="s">
-        <v>194</v>
+        <v>94</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>195</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>196</v>
+        <v>175</v>
+      </c>
+      <c r="B82" t="s">
+        <v>176</v>
       </c>
       <c r="C82" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>190</v>
+      </c>
+      <c r="B83" t="s">
+        <v>191</v>
+      </c>
+      <c r="C83" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>193</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C84" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>197</v>
+      </c>
+      <c r="B85" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" t="s">
         <v>199</v>
       </c>
-      <c r="B83" t="s">
-        <v>200</v>
-      </c>
-      <c r="C83" t="s">
-        <v>201</v>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>257</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prompt for OUs using custom input
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D00DB5-ABC0-40FD-9411-3C92BD5A9141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD63172-9928-4931-A3C7-99CF80209FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="267">
   <si>
     <t>Name</t>
   </si>
@@ -300,12 +300,6 @@
     <t>RobotNotFound</t>
   </si>
   <si>
-    <t>ChooseOUMessage</t>
-  </si>
-  <si>
-    <t>ChooseOUTitle</t>
-  </si>
-  <si>
     <t>OUNotFound</t>
   </si>
   <si>
@@ -321,18 +315,9 @@
     <t>EnvironmentNotFound</t>
   </si>
   <si>
-    <t>Choose Organization Unit</t>
-  </si>
-  <si>
     <t>組織単位を選択してください。</t>
   </si>
   <si>
-    <t>組織単位</t>
-  </si>
-  <si>
-    <t>Organization Unit</t>
-  </si>
-  <si>
     <t>CreateAssetIDColumn</t>
   </si>
   <si>
@@ -832,6 +817,24 @@
   </si>
   <si>
     <t>Misc\Forms\AuthenticationPanel.html</t>
+  </si>
+  <si>
+    <t>OrganizationUnitsPanelTemplatePath</t>
+  </si>
+  <si>
+    <t>OrganizationUnitsPanelPath</t>
+  </si>
+  <si>
+    <t>Misc\Forms\OrganizationUnitsPanelTemplate.html</t>
+  </si>
+  <si>
+    <t>Misc\Forms\OrganizationUnitsPanel.html</t>
+  </si>
+  <si>
+    <t>FormChooseOUMessage</t>
+  </si>
+  <si>
+    <t>Please choose the Organization Units.</t>
   </si>
 </sst>
 </file>
@@ -908,8 +911,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C29" totalsRowShown="0">
-  <autoFilter ref="A1:C29" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0">
+  <autoFilter ref="A1:C31" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -920,8 +923,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C87" totalsRowShown="0">
-  <autoFilter ref="A1:C87" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C86" totalsRowShown="0">
+  <autoFilter ref="A1:C86" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1194,9 +1197,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1223,15 +1226,15 @@
         <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1252,63 +1255,63 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="B8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="B9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>239</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
@@ -1316,95 +1319,95 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>256</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
         <v>74</v>
@@ -1412,33 +1415,49 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>196</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1453,9 +1472,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1479,51 +1498,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>20</v>
@@ -1534,7 +1553,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -1545,363 +1564,363 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>188</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>189</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="A21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>201</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>207</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>202</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>251</v>
+        <v>196</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>250</v>
+        <v>202</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>252</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="A28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>112</v>
@@ -1909,337 +1928,337 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>133</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="A54" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>160</v>
+        <v>204</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>206</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>211</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="A61" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>203</v>
+        <v>144</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>176</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>204</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>206</v>
-      </c>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="A71" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>168</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -2247,87 +2266,76 @@
         <v>130</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>135</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>136</v>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>94</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>106</v>
+        <v>170</v>
+      </c>
+      <c r="B81" t="s">
+        <v>171</v>
+      </c>
+      <c r="C81" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="C82" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" t="s">
         <v>190</v>
-      </c>
-      <c r="B83" t="s">
-        <v>191</v>
-      </c>
-      <c r="C83" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>192</v>
+      </c>
+      <c r="B84" t="s">
         <v>193</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" t="s">
         <v>194</v>
-      </c>
-      <c r="C84" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>197</v>
-      </c>
-      <c r="B85" t="s">
-        <v>198</v>
-      </c>
-      <c r="C85" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>257</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optionally receive language as argument
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA35E749-268D-46AC-9A3E-297B79589023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52849905-06B2-4116-90B4-6C85A3960BB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="275">
   <si>
     <t>Name</t>
   </si>
@@ -853,6 +853,12 @@
   </si>
   <si>
     <t>プロセス</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Two-letter ISO code of language to be used by the tool. Currently supported languages: EN, JA.</t>
   </si>
 </sst>
 </file>
@@ -908,7 +914,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -929,12 +938,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0">
-  <autoFilter ref="A1:C31" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0">
+  <autoFilter ref="A1:C32" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
-    <tableColumn id="3" xr3:uid="{913515CE-4C01-4C71-A47B-9737010FF509}" name="Explanation"/>
+    <tableColumn id="3" xr3:uid="{913515CE-4C01-4C71-A47B-9737010FF509}" name="Explanation" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1215,9 +1224,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1225,7 +1234,7 @@
   <cols>
     <col min="1" max="1" width="39.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59" customWidth="1"/>
+    <col min="3" max="3" width="62.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1246,6 +1255,7 @@
       <c r="B2" s="2" t="s">
         <v>255</v>
       </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1254,6 +1264,7 @@
       <c r="B3" t="s">
         <v>256</v>
       </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1262,6 +1273,7 @@
       <c r="B4">
         <v>200</v>
       </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1270,214 +1282,252 @@
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>273</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
-        <v>258</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
-        <v>263</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="B10" t="s">
-        <v>259</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>94</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>66</v>
-      </c>
-      <c r="B17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>68</v>
       </c>
       <c r="B18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>69</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>95</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>75</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>78</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>84</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>89</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>85</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>179</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>191</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>180</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>181</v>
-      </c>
-      <c r="B30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>195</v>
       </c>
       <c r="B31" t="s">
         <v>38</v>
       </c>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>195</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1492,7 +1542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Properly display forms with 100% zoom
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52849905-06B2-4116-90B4-6C85A3960BB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB3E61-07A9-4E38-9273-4574FDB9D760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="277">
   <si>
     <t>Name</t>
   </si>
@@ -855,10 +855,16 @@
     <t>プロセス</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Two-letter ISO code of language to be used by the tool. Currently supported languages: EN, JA.</t>
+    <t>EntitiesWorkbooksFolder</t>
+  </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <t>FormsHeight</t>
+  </si>
+  <si>
+    <t>FormsWidth</t>
   </si>
 </sst>
 </file>
@@ -938,8 +944,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0">
-  <autoFilter ref="A1:C32" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C34" totalsRowShown="0">
+  <autoFilter ref="A1:C34" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -1224,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1268,117 +1274,115 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>200</v>
+        <v>273</v>
+      </c>
+      <c r="B4" t="s">
+        <v>274</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>273</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>274</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>211</v>
-      </c>
-      <c r="B7" t="s">
-        <v>257</v>
+        <v>275</v>
+      </c>
+      <c r="B7">
+        <v>400</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" t="s">
-        <v>258</v>
+        <v>276</v>
+      </c>
+      <c r="B8">
+        <v>500</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="B10" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="B11" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>239</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>259</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>260</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>43</v>
@@ -1387,106 +1391,106 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>251</v>
+        <v>76</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>251</v>
       </c>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
         <v>74</v>
@@ -1495,39 +1499,57 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>191</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>195</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Include additional logging and reorganize project files
Log what operation is performed on what entity.
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB3E61-07A9-4E38-9273-4574FDB9D760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588E5BFA-3587-46E2-AED0-2A3ADDA96B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="280">
   <si>
     <t>Name</t>
   </si>
@@ -549,9 +549,6 @@
     <t>RobotEnvironmentAssociationFailure</t>
   </si>
   <si>
-    <t>Failed to add robot to environment.　Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
     <t>ロボットをロボットグループに追加することができませんでした。リクエストステータス：{0} / レスポンス：{1}。</t>
   </si>
   <si>
@@ -865,6 +862,18 @@
   </si>
   <si>
     <t>FormsWidth</t>
+  </si>
+  <si>
+    <t>Failed to add robot to environment. Request status: {0} / Response: {1}.</t>
+  </si>
+  <si>
+    <t>StartProcessingEntity</t>
+  </si>
+  <si>
+    <t>Starting to {0} {1}.</t>
+  </si>
+  <si>
+    <t>{1}の{0}を開始します。</t>
   </si>
 </sst>
 </file>
@@ -956,8 +965,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C88" totalsRowShown="0">
-  <autoFilter ref="A1:C88" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C89" totalsRowShown="0">
+  <autoFilter ref="A1:C89" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1232,7 +1241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1259,25 +1268,25 @@
         <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" t="s">
         <v>273</v>
-      </c>
-      <c r="B4" t="s">
-        <v>274</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1301,7 +1310,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -1310,7 +1319,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B8">
         <v>500</v>
@@ -1319,55 +1328,55 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -1475,7 +1484,7 @@
         <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -1508,7 +1517,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
         <v>74</v>
@@ -1517,7 +1526,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B31" t="s">
         <v>43</v>
@@ -1526,7 +1535,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" t="s">
         <v>47</v>
@@ -1535,7 +1544,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
         <v>38</v>
@@ -1544,7 +1553,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
         <v>38</v>
@@ -1562,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,51 +1597,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>20</v>
@@ -1643,7 +1652,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -1654,98 +1663,98 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>264</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>93</v>
@@ -1801,24 +1810,24 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>266</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1871,24 +1880,24 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -2191,24 +2200,24 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -2220,7 +2229,7 @@
         <v>82</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>83</v>
@@ -2272,35 +2281,35 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>172</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>175</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>198</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -2400,54 +2409,65 @@
         <v>170</v>
       </c>
       <c r="B83" t="s">
+        <v>276</v>
+      </c>
+      <c r="C83" t="s">
         <v>171</v>
-      </c>
-      <c r="C83" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>184</v>
+      </c>
+      <c r="B84" t="s">
         <v>185</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>186</v>
-      </c>
-      <c r="C84" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>187</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="C85" t="s">
         <v>189</v>
-      </c>
-      <c r="C85" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>191</v>
+      </c>
+      <c r="B86" t="s">
         <v>192</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>193</v>
-      </c>
-      <c r="C86" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>251</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>253</v>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>277</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Confirm whether roles exists before assigning them to users
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588E5BFA-3587-46E2-AED0-2A3ADDA96B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9399E476-4ADF-44CF-9CBC-F802B3A99063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="283">
   <si>
     <t>Name</t>
   </si>
@@ -798,12 +798,6 @@
     <t>A robot is being added and removed at the same time.</t>
   </si>
   <si>
-    <t>https://platform.uipath.com</t>
-  </si>
-  <si>
-    <t>MateusTenant</t>
-  </si>
-  <si>
     <t>Misc\Forms\ControlPanelTemplate.html</t>
   </si>
   <si>
@@ -874,6 +868,21 @@
   </si>
   <si>
     <t>{1}の{0}を開始します。</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>https://win-9d2vvsqpta7</t>
+  </si>
+  <si>
+    <t>RoleNotFound</t>
+  </si>
+  <si>
+    <t>Role not found.</t>
+  </si>
+  <si>
+    <t>ロールが見つかりませんでした。</t>
   </si>
 </sst>
 </file>
@@ -965,8 +974,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C89" totalsRowShown="0">
-  <autoFilter ref="A1:C89" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C91" totalsRowShown="0">
+  <autoFilter ref="A1:C91" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1242,7 +1251,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1268,7 +1277,7 @@
         <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1277,16 +1286,16 @@
         <v>240</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1310,7 +1319,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -1319,7 +1328,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B8">
         <v>500</v>
@@ -1331,7 +1340,7 @@
         <v>210</v>
       </c>
       <c r="B9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1340,25 +1349,25 @@
         <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" t="s">
         <v>260</v>
-      </c>
-      <c r="B11" t="s">
-        <v>262</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B12" t="s">
         <v>261</v>
-      </c>
-      <c r="B12" t="s">
-        <v>263</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -1367,7 +1376,7 @@
         <v>238</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -1376,7 +1385,7 @@
         <v>239</v>
       </c>
       <c r="B14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -1561,20 +1570,23 @@
       <c r="C34" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9ECA3495-0800-4646-B856-23005494606C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1718,13 +1730,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>267</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1751,10 +1763,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>93</v>
@@ -1821,13 +1833,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2409,7 +2421,7 @@
         <v>170</v>
       </c>
       <c r="B83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C83" t="s">
         <v>171</v>
@@ -2461,13 +2473,28 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>280</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>275</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor workflows that get IDs based on names of entities
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9399E476-4ADF-44CF-9CBC-F802B3A99063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B74BD1B-940A-4E2F-B78B-5DF41753DDDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="299">
   <si>
     <t>Name</t>
   </si>
@@ -795,9 +795,6 @@
     <t>ロボットが同時に追加・削除されています。</t>
   </si>
   <si>
-    <t>A robot is being added and removed at the same time.</t>
-  </si>
-  <si>
     <t>Misc\Forms\ControlPanelTemplate.html</t>
   </si>
   <si>
@@ -883,6 +880,57 @@
   </si>
   <si>
     <t>ロールが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>NamedOUNotFound</t>
+  </si>
+  <si>
+    <t>Organization Unit named {0} not found.</t>
+  </si>
+  <si>
+    <t>{0}という組織単位が見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>NamedRoleNotFound</t>
+  </si>
+  <si>
+    <t>Role named {0} not found.</t>
+  </si>
+  <si>
+    <t>{0}というロールが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>OUAddedAndRemoved</t>
+  </si>
+  <si>
+    <t>An Organization Unit is being added and removed at the same time.</t>
+  </si>
+  <si>
+    <t>組織単位が同時に追加・削除されています。</t>
+  </si>
+  <si>
+    <t>A Robot is being added and removed at the same time.</t>
+  </si>
+  <si>
+    <t>AddRemoveOrganizationUnitsResultColumn</t>
+  </si>
+  <si>
+    <t>Assign Organization Units</t>
+  </si>
+  <si>
+    <t>AssignOrganizationUnitsOperationName</t>
+  </si>
+  <si>
+    <t>組織単位の設定</t>
+  </si>
+  <si>
+    <t>NamedMachineNotFound</t>
+  </si>
+  <si>
+    <t>Machine named {0} not found.</t>
+  </si>
+  <si>
+    <t>{0}というマシンが見つかりませんでした。</t>
   </si>
 </sst>
 </file>
@@ -962,8 +1010,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C34" totalsRowShown="0">
-  <autoFilter ref="A1:C34" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C35" totalsRowShown="0">
+  <autoFilter ref="A1:C35" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -974,8 +1022,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C91" totalsRowShown="0">
-  <autoFilter ref="A1:C91" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C95" totalsRowShown="0">
+  <autoFilter ref="A1:C95" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1248,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1277,7 +1325,7 @@
         <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1286,16 +1334,16 @@
         <v>240</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" t="s">
         <v>270</v>
-      </c>
-      <c r="B4" t="s">
-        <v>271</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1319,7 +1367,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -1328,7 +1376,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B8">
         <v>500</v>
@@ -1340,7 +1388,7 @@
         <v>210</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1349,25 +1397,25 @@
         <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -1376,7 +1424,7 @@
         <v>238</v>
       </c>
       <c r="B13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -1385,7 +1433,7 @@
         <v>239</v>
       </c>
       <c r="B14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -1568,6 +1616,15 @@
         <v>38</v>
       </c>
       <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1583,15 +1640,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79" customWidth="1"/>
     <col min="3" max="3" width="114.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1730,13 +1787,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1763,10 +1820,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>93</v>
@@ -1833,13 +1890,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>263</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1903,598 +1960,653 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>294</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>245</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>114</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>104</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-    </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>63</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>128</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-    </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>205</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>288</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>197</v>
+        <v>289</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>83</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>87</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>87</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>162</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>175</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>198</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-    </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>86</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>57</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>163</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>296</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>97</v>
+        <v>297</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>119</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>121</v>
+        <v>298</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>170</v>
-      </c>
-      <c r="B83" t="s">
-        <v>274</v>
-      </c>
-      <c r="C83" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>184</v>
-      </c>
-      <c r="B84" t="s">
-        <v>185</v>
-      </c>
-      <c r="C84" t="s">
-        <v>186</v>
+        <v>282</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>187</v>
+        <v>92</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C85" t="s">
-        <v>189</v>
+        <v>169</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B86" t="s">
-        <v>192</v>
+        <v>273</v>
       </c>
       <c r="C86" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>251</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>252</v>
+        <v>184</v>
+      </c>
+      <c r="B87" t="s">
+        <v>185</v>
+      </c>
+      <c r="C87" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>187</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>191</v>
+      </c>
+      <c r="B89" t="s">
+        <v>192</v>
+      </c>
+      <c r="C89" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>251</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>279</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>285</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>274</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement AddRemoveUserOrganizationUnits and related workflows
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B74BD1B-940A-4E2F-B78B-5DF41753DDDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788D0075-6922-4ECD-8465-B87F1E679FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="302">
   <si>
     <t>Name</t>
   </si>
@@ -915,15 +915,6 @@
     <t>AddRemoveOrganizationUnitsResultColumn</t>
   </si>
   <si>
-    <t>Assign Organization Units</t>
-  </si>
-  <si>
-    <t>AssignOrganizationUnitsOperationName</t>
-  </si>
-  <si>
-    <t>組織単位の設定</t>
-  </si>
-  <si>
     <t>NamedMachineNotFound</t>
   </si>
   <si>
@@ -931,6 +922,24 @@
   </si>
   <si>
     <t>{0}というマシンが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>NamedUserNotFound</t>
+  </si>
+  <si>
+    <t>Username {0} not found.</t>
+  </si>
+  <si>
+    <t>{0}というユーザー名が見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>AddRemoveOrganizationUnitsOperationName</t>
+  </si>
+  <si>
+    <t>Add Or Remove Organization Units</t>
+  </si>
+  <si>
+    <t>組織単位の追加・削除</t>
   </si>
 </sst>
 </file>
@@ -1022,8 +1031,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C95" totalsRowShown="0">
-  <autoFilter ref="A1:C95" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C96" totalsRowShown="0">
+  <autoFilter ref="A1:C96" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1298,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1640,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1960,13 +1969,13 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -2312,300 +2321,311 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="A64" t="s">
+        <v>296</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>159</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>175</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>198</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-    </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>86</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>163</v>
+        <v>57</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>164</v>
+        <v>58</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>165</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>296</v>
+        <v>163</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>297</v>
+        <v>164</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>88</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>98</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>293</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>282</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>92</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>170</v>
-      </c>
-      <c r="B86" t="s">
-        <v>273</v>
-      </c>
-      <c r="C86" t="s">
-        <v>171</v>
+        <v>92</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B87" t="s">
-        <v>185</v>
+        <v>273</v>
       </c>
       <c r="C87" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>187</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
+      </c>
+      <c r="B88" t="s">
+        <v>185</v>
       </c>
       <c r="C88" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>191</v>
-      </c>
-      <c r="B89" t="s">
-        <v>192</v>
+        <v>187</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="C89" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>191</v>
+      </c>
+      <c r="B90" t="s">
+        <v>192</v>
+      </c>
+      <c r="C90" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>251</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>279</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>279</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>285</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-    </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>274</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement AddRemoveUserRoles and related workflows
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788D0075-6922-4ECD-8465-B87F1E679FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E140F1C5-3F4E-4DA3-A08E-2B86B1A83ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="298">
   <si>
     <t>Name</t>
   </si>
@@ -72,27 +72,6 @@
     <t>削除</t>
   </si>
   <si>
-    <t>ChooseEntityMessage</t>
-  </si>
-  <si>
-    <t>Choose entity to operate.</t>
-  </si>
-  <si>
-    <t>エンティティを選択してください。</t>
-  </si>
-  <si>
-    <t>ChooseEntityTitle</t>
-  </si>
-  <si>
-    <t>ChooseOperationMessage</t>
-  </si>
-  <si>
-    <t>ChooseOperationTitle</t>
-  </si>
-  <si>
-    <t>Choose operation to perform.</t>
-  </si>
-  <si>
     <t>Operation</t>
   </si>
   <si>
@@ -102,9 +81,6 @@
     <t>エンティティ</t>
   </si>
   <si>
-    <t>操作を選択してください。</t>
-  </si>
-  <si>
     <t>操作</t>
   </si>
   <si>
@@ -858,15 +834,6 @@
     <t>Failed to add robot to environment. Request status: {0} / Response: {1}.</t>
   </si>
   <si>
-    <t>StartProcessingEntity</t>
-  </si>
-  <si>
-    <t>Starting to {0} {1}.</t>
-  </si>
-  <si>
-    <t>{1}の{0}を開始します。</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -936,10 +903,31 @@
     <t>AddRemoveOrganizationUnitsOperationName</t>
   </si>
   <si>
-    <t>Add Or Remove Organization Units</t>
-  </si>
-  <si>
     <t>組織単位の追加・削除</t>
+  </si>
+  <si>
+    <t>AddRemoveRolesOperationName</t>
+  </si>
+  <si>
+    <t>Add Or Remove Roles</t>
+  </si>
+  <si>
+    <t>ロールの追加・削除</t>
+  </si>
+  <si>
+    <t>AddRemoveRolesResultColumn</t>
+  </si>
+  <si>
+    <t>RoleAddedAndRemoved</t>
+  </si>
+  <si>
+    <t>A Role is being added and removed at the same time.</t>
+  </si>
+  <si>
+    <t>ロールが同時に追加・削除されています。</t>
+  </si>
+  <si>
+    <t>Add Or Remove Ous</t>
   </si>
 </sst>
 </file>
@@ -1019,8 +1007,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C35" totalsRowShown="0">
-  <autoFilter ref="A1:C35" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0">
+  <autoFilter ref="A1:C36" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -1031,8 +1019,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C96" totalsRowShown="0">
-  <autoFilter ref="A1:C96" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C92" totalsRowShown="0">
+  <autoFilter ref="A1:C92" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1305,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1326,39 +1314,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -1367,7 +1355,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1376,7 +1364,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -1385,7 +1373,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B8">
         <v>500</v>
@@ -1394,246 +1382,255 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B9" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B10" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1649,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1675,167 +1672,167 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1844,68 +1841,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1914,7 +1911,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
@@ -1925,7 +1922,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
@@ -1936,7 +1933,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
@@ -1947,7 +1944,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
@@ -1958,674 +1955,637 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>245</v>
+        <v>290</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>244</v>
+        <v>291</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>246</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="A32" t="s">
+        <v>237</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>135</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>139</v>
+        <v>56</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>142</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
+      <c r="A50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>116</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>194</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>152</v>
+        <v>198</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>153</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>277</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>155</v>
+        <v>278</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>156</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>202</v>
+        <v>294</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>203</v>
+        <v>295</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>204</v>
+        <v>296</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>206</v>
+        <v>286</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>207</v>
+        <v>287</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>288</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>290</v>
-      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>296</v>
+        <v>74</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>297</v>
+        <v>189</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>298</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>197</v>
+        <v>150</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>175</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>177</v>
-      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>198</v>
+        <v>78</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>199</v>
+        <v>135</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>200</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="A74" t="s">
+        <v>49</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>282</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>58</v>
+        <v>283</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>163</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>165</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>294</v>
+        <v>89</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>295</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>125</v>
+        <v>271</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>126</v>
+        <v>272</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>130</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>131</v>
+        <v>273</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>282</v>
+        <v>84</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>283</v>
+        <v>161</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>284</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" t="s">
+        <v>265</v>
+      </c>
+      <c r="C85" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>92</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>101</v>
+        <v>176</v>
+      </c>
+      <c r="B86" t="s">
+        <v>177</v>
+      </c>
+      <c r="C86" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>170</v>
-      </c>
-      <c r="B87" t="s">
-        <v>273</v>
+        <v>179</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="C87" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>183</v>
+      </c>
+      <c r="B88" t="s">
         <v>184</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>185</v>
-      </c>
-      <c r="C88" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C89" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>191</v>
-      </c>
-      <c r="B90" t="s">
-        <v>192</v>
-      </c>
-      <c r="C90" t="s">
-        <v>193</v>
+        <v>280</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>279</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>285</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>274</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement CreateProcess and DeleteProcess workflows
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E140F1C5-3F4E-4DA3-A08E-2B86B1A83ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD178442-0646-4159-957B-1F92EB4CCDA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="319">
   <si>
     <t>Name</t>
   </si>
@@ -928,6 +928,69 @@
   </si>
   <si>
     <t>Add Or Remove Ous</t>
+  </si>
+  <si>
+    <t>ProcessNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Process name not specified.</t>
+  </si>
+  <si>
+    <t>プロセス名が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>PackageNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Package name not specified.</t>
+  </si>
+  <si>
+    <t>パッケージ名が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>CreateProcessResultColumn</t>
+  </si>
+  <si>
+    <t>CreateProcessIDColumn</t>
+  </si>
+  <si>
+    <t>PackageVersionNotSpecified</t>
+  </si>
+  <si>
+    <t>Package version not specified</t>
+  </si>
+  <si>
+    <t>パッケージバージョンが指定されませんでした。</t>
+  </si>
+  <si>
+    <t>ProcessIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Process ID invalid or not specified.</t>
+  </si>
+  <si>
+    <t>プロセスIDが無効か指定されませんでした。</t>
+  </si>
+  <si>
+    <t>ProcessNotFound</t>
+  </si>
+  <si>
+    <t>Process not found.</t>
+  </si>
+  <si>
+    <t>プロセスが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>ProcessIDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Process ID and Process name do not match.</t>
+  </si>
+  <si>
+    <t>指定されたプロセス名とプロセスIDが一致しません。</t>
+  </si>
+  <si>
+    <t>DeleteProcessResultColumn</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1070,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0">
-  <autoFilter ref="A1:C36" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C39" totalsRowShown="0">
+  <autoFilter ref="A1:C39" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -1019,8 +1082,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C92" totalsRowShown="0">
-  <autoFilter ref="A1:C92" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C100" totalsRowShown="0">
+  <autoFilter ref="A1:C100" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1293,7 +1356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1632,6 +1695,33 @@
       </c>
       <c r="C36" s="1"/>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>305</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>304</v>
+      </c>
+      <c r="B38" t="s">
+        <v>242</v>
+      </c>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>318</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{9ECA3495-0800-4646-B856-23005494606C}"/>
@@ -1646,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2589,6 +2679,80 @@
         <v>276</v>
       </c>
     </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>298</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>309</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>312</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>315</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>301</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>306</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add explanations about settings
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD178442-0646-4159-957B-1F92EB4CCDA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE00F1-B27B-46E5-9280-C4C48D8C9F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="LocalizedSettings" sheetId="2" r:id="rId2"/>
+    <sheet name="Settings" sheetId="3" r:id="rId1"/>
+    <sheet name="Advanced Settings" sheetId="1" r:id="rId2"/>
+    <sheet name="Localization" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="354">
   <si>
     <t>Name</t>
   </si>
@@ -756,9 +757,6 @@
     <t>FormAccountLockoutWarning</t>
   </si>
   <si>
-    <t>Please mind that many unncessful login attempts can temporarily lock the account, as specified in the Security settings of the tenant.</t>
-  </si>
-  <si>
     <t>テナントの設定により、ログイン試行に複数回失敗した場合、アカウントを指定された秒数の間ロックされることご注意ください。</t>
   </si>
   <si>
@@ -819,12 +817,6 @@
     <t>プロセス</t>
   </si>
   <si>
-    <t>EntitiesWorkbooksFolder</t>
-  </si>
-  <si>
-    <t>Config</t>
-  </si>
-  <si>
     <t>FormsHeight</t>
   </si>
   <si>
@@ -834,12 +826,6 @@
     <t>Failed to add robot to environment. Request status: {0} / Response: {1}.</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>https://win-9d2vvsqpta7</t>
-  </si>
-  <si>
     <t>RoleNotFound</t>
   </si>
   <si>
@@ -879,9 +865,6 @@
     <t>A Robot is being added and removed at the same time.</t>
   </si>
   <si>
-    <t>AddRemoveOrganizationUnitsResultColumn</t>
-  </si>
-  <si>
     <t>NamedMachineNotFound</t>
   </si>
   <si>
@@ -915,9 +898,6 @@
     <t>ロールの追加・削除</t>
   </si>
   <si>
-    <t>AddRemoveRolesResultColumn</t>
-  </si>
-  <si>
     <t>RoleAddedAndRemoved</t>
   </si>
   <si>
@@ -927,9 +907,6 @@
     <t>ロールが同時に追加・削除されています。</t>
   </si>
   <si>
-    <t>Add Or Remove Ous</t>
-  </si>
-  <si>
     <t>ProcessNameNotSpecified</t>
   </si>
   <si>
@@ -991,6 +968,136 @@
   </si>
   <si>
     <t>DeleteProcessResultColumn</t>
+  </si>
+  <si>
+    <t>URL of the Orchestrator instance to be used.</t>
+  </si>
+  <si>
+    <t>Name of the tenant to be used.</t>
+  </si>
+  <si>
+    <t>Height of the window used to show forms.</t>
+  </si>
+  <si>
+    <t>Width of the window used to show forms.</t>
+  </si>
+  <si>
+    <t>Path to the file to be used as Control Panel form.</t>
+  </si>
+  <si>
+    <t>Path to the template file used to generate the Control Panel form.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interval (in milliseconds) between operations on entities. This can be used to control the impact on Orchestrator's infrastructure. </t>
+  </si>
+  <si>
+    <t>Maximum number of requests that should be allowed to be made at once in one run. This can be used to control the impact on Orchestrator's infrastructure. 
+Note, however, that some entities make more than one request per operation. For instance, to delete an asset, the Orchestrator manager makes additional requests to confirm data about the specified Organization Unit and Asset.</t>
+  </si>
+  <si>
+    <t>Path to the file to be used as Organization Units Panel form.</t>
+  </si>
+  <si>
+    <t>Path to the template file used to generate the Organization Units Panel form.</t>
+  </si>
+  <si>
+    <t>Path to the template file used to generate the Authentication Panel form.</t>
+  </si>
+  <si>
+    <t>Path to the file to be used as Authentication Panel form.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Machine operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Asset operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Machine operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Asset operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Edit Asset operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create User operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the Key of the created Machine should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the ID of the created Machine should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the ID of the created Asset should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete User operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Edit User operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Robot operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Robot operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Edit Robot operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the ID of the created User should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Environment operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Environment operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Process operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Process operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the ID of the created Environment should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the ID of the created Process should be written.</t>
+  </si>
+  <si>
+    <t>AddRemoveUserOrganizationUnitsResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Add Remove User's Organization Units operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Add Remove Environment's Robots operation should be written.</t>
+  </si>
+  <si>
+    <t>AddRemoveUserRolesResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Add Remove User's Roles operation should be written.</t>
+  </si>
+  <si>
+    <t>Column to which the ID of the created Robot should be written.</t>
+  </si>
+  <si>
+    <t>Please mind that many unsuccessful login attempts can temporarily lock the account, as specified in the Security settings of the tenant.</t>
+  </si>
+  <si>
+    <t>Add Or Remove OUs</t>
+  </si>
+  <si>
+    <t>https://platform.uipath.com</t>
+  </si>
+  <si>
+    <t>MateusTenant</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1153,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1070,8 +1180,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C39" totalsRowShown="0">
-  <autoFilter ref="A1:C39" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7F8F45FE-2B96-4F08-8C9F-E71B4ACCE2FA}" name="Table14" displayName="Table14" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D8D5B6DE-5265-4940-BA42-B3804FA368B2}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{040BFB8F-6ACC-4B54-BAD6-564D9FD4EC4E}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{6C5EAD48-5E0B-44E0-B023-F34A656E492B}" name="Explanation" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0">
+  <autoFilter ref="A1:C36" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -1081,7 +1203,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C100" totalsRowShown="0">
   <autoFilter ref="A1:C100" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
@@ -1355,8 +1477,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1385,346 +1507,26 @@
         <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>352</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>232</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
-        <v>200</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>263</v>
-      </c>
-      <c r="B7">
-        <v>400</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>264</v>
-      </c>
-      <c r="B8">
-        <v>500</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B10" t="s">
-        <v>246</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>249</v>
-      </c>
-      <c r="B11" t="s">
-        <v>251</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>250</v>
-      </c>
-      <c r="B12" t="s">
-        <v>252</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>230</v>
-      </c>
-      <c r="B13" t="s">
-        <v>247</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>231</v>
-      </c>
-      <c r="B14" t="s">
-        <v>248</v>
-      </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" t="s">
-        <v>242</v>
-      </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>170</v>
-      </c>
-      <c r="B30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>182</v>
-      </c>
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>186</v>
-      </c>
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>281</v>
-      </c>
-      <c r="B35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>293</v>
-      </c>
-      <c r="B36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>305</v>
-      </c>
-      <c r="B37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>304</v>
-      </c>
-      <c r="B38" t="s">
-        <v>242</v>
-      </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>318</v>
-      </c>
-      <c r="B39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="1"/>
+        <v>353</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>312</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{9ECA3495-0800-4646-B856-23005494606C}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{962F7B28-6511-4D72-8544-E32A44E6812C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1735,11 +1537,431 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5">
+        <v>500</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>344</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>347</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>297</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>296</v>
+      </c>
+      <c r="B35" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>310</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1776,10 +1998,10 @@
         <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1883,13 +2105,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1916,10 +2138,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>85</v>
@@ -1986,13 +2208,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>254</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2056,24 +2278,24 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>297</v>
+        <v>351</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -2365,35 +2587,35 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -2527,13 +2749,13 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -2582,13 +2804,13 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -2607,7 +2829,7 @@
         <v>162</v>
       </c>
       <c r="B85" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C85" t="s">
         <v>163</v>
@@ -2648,35 +2870,35 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>242</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -2685,46 +2907,46 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -2733,24 +2955,24 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separate create/edit credential Assets from regular Assets
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE00F1-B27B-46E5-9280-C4C48D8C9F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313EBB62-B5AB-427E-BACB-C083C3EC7B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="374">
   <si>
     <t>Name</t>
   </si>
@@ -598,9 +598,6 @@
     <t>AddRemoveEnvironmentRobotsResultColumn</t>
   </si>
   <si>
-    <t>AddRemoveRobotsOperationName</t>
-  </si>
-  <si>
     <t>ロボットの追加・削除</t>
   </si>
   <si>
@@ -883,13 +880,7 @@
     <t>{0}というユーザー名が見つかりませんでした。</t>
   </si>
   <si>
-    <t>AddRemoveOrganizationUnitsOperationName</t>
-  </si>
-  <si>
     <t>組織単位の追加・削除</t>
-  </si>
-  <si>
-    <t>AddRemoveRolesOperationName</t>
   </si>
   <si>
     <t>Add Or Remove Roles</t>
@@ -1094,10 +1085,79 @@
     <t>Add Or Remove OUs</t>
   </si>
   <si>
-    <t>https://platform.uipath.com</t>
-  </si>
-  <si>
-    <t>MateusTenant</t>
+    <t>AddRemoveUserOrganizationUnitsOperationName</t>
+  </si>
+  <si>
+    <t>AddRemoveUserRolesOperationName</t>
+  </si>
+  <si>
+    <t>AddRemoveEnvironmentRobotsOperationName</t>
+  </si>
+  <si>
+    <t>InvalidAssetValue</t>
+  </si>
+  <si>
+    <t>無効な値が指定されました。</t>
+  </si>
+  <si>
+    <t>Invalid value.</t>
+  </si>
+  <si>
+    <t>https://win-9d2vvsqpta7/</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>ユーザー名の編集に新しいパスワードが必要です。</t>
+  </si>
+  <si>
+    <t>New Password required when changing Username.</t>
+  </si>
+  <si>
+    <t>EditCredentialUsernameNewPasswordRequired</t>
+  </si>
+  <si>
+    <t>PasswordNotSpecified</t>
+  </si>
+  <si>
+    <t>Password not specified.</t>
+  </si>
+  <si>
+    <t>パスワードが指定されませんでした。</t>
+  </si>
+  <si>
+    <t>CreateCredentialOperationName</t>
+  </si>
+  <si>
+    <t>EditCredentialOperationName</t>
+  </si>
+  <si>
+    <t>Create Credential</t>
+  </si>
+  <si>
+    <t>Edit Credential</t>
+  </si>
+  <si>
+    <t>Credential型の作成</t>
+  </si>
+  <si>
+    <t>Credential型の編集</t>
+  </si>
+  <si>
+    <t>CreateCredentialAssetResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Credential Asset operation should be written.</t>
+  </si>
+  <si>
+    <t>EditCredentialAssetResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Edit Credential Asset operation should be written.</t>
+  </si>
+  <si>
+    <t>CreateCredentialAssetIDColumn</t>
   </si>
 </sst>
 </file>
@@ -1192,8 +1252,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0">
-  <autoFilter ref="A1:C36" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C39" totalsRowShown="0">
+  <autoFilter ref="A1:C39" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -1204,8 +1264,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C100" totalsRowShown="0">
-  <autoFilter ref="A1:C100" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C105" totalsRowShown="0">
+  <autoFilter ref="A1:C105" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1507,26 +1567,26 @@
         <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{962F7B28-6511-4D72-8544-E32A44E6812C}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{7B9ACE39-67E0-4AAE-B10F-7C3353C799CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1538,7 +1598,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1570,7 +1630,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1581,95 +1641,95 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B4">
         <v>400</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B5">
         <v>500</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1680,7 +1740,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1691,7 +1751,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1702,7 +1762,7 @@
         <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1713,7 +1773,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1724,7 +1784,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1735,191 +1795,191 @@
         <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>373</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>369</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>324</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>371</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>328</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>241</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>240</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>76</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>170</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>339</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>186</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>344</v>
+        <v>171</v>
       </c>
       <c r="B32" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>347</v>
+        <v>172</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>297</v>
+        <v>186</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>343</v>
@@ -1927,24 +1987,57 @@
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>296</v>
+        <v>341</v>
       </c>
       <c r="B35" t="s">
-        <v>241</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>310</v>
+        <v>344</v>
       </c>
       <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>294</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>293</v>
+      </c>
+      <c r="B38" t="s">
+        <v>240</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>307</v>
+      </c>
+      <c r="B39" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>341</v>
+      <c r="C39" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -1958,15 +2051,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79" customWidth="1"/>
     <col min="3" max="3" width="114.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1984,51 +2077,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -2039,7 +2132,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -2050,98 +2143,98 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>85</v>
@@ -2208,13 +2301,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2267,686 +2360,693 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>187</v>
+        <v>363</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>193</v>
+        <v>365</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>188</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>282</v>
+        <v>364</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>283</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>284</v>
+        <v>351</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>285</v>
+        <v>192</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>286</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>237</v>
+        <v>349</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>236</v>
+        <v>348</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>238</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="A33" t="s">
+        <v>350</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>236</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>235</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>28</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="A47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="A53" t="s">
+        <v>114</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>140</v>
+        <v>352</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>141</v>
+        <v>354</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>142</v>
+        <v>353</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>359</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>144</v>
+        <v>358</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>145</v>
+        <v>357</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>146</v>
+        <v>360</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>147</v>
+        <v>361</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>148</v>
+        <v>362</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>194</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>196</v>
-      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>197</v>
+        <v>137</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>198</v>
+        <v>138</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>199</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>272</v>
+        <v>140</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>273</v>
+        <v>141</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>274</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>287</v>
+        <v>143</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>288</v>
+        <v>144</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>289</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>279</v>
+        <v>146</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>280</v>
+        <v>147</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>281</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="A63" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>271</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>136</v>
+        <v>272</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>91</v>
+        <v>273</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>284</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>150</v>
+        <v>285</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>151</v>
+        <v>286</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>152</v>
+        <v>278</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>153</v>
+        <v>279</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>154</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>158</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>160</v>
-      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>164</v>
+        <v>74</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>166</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>169</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="A72" t="s">
+        <v>152</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>50</v>
+        <v>165</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>276</v>
+        <v>189</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>277</v>
+        <v>190</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>278</v>
-      </c>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>122</v>
+        <v>275</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>124</v>
+        <v>276</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>266</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>268</v>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>162</v>
-      </c>
-      <c r="B85" t="s">
-        <v>262</v>
-      </c>
-      <c r="C85" t="s">
-        <v>163</v>
+        <v>117</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>176</v>
-      </c>
-      <c r="B86" t="s">
-        <v>177</v>
-      </c>
-      <c r="C86" t="s">
-        <v>178</v>
+        <v>122</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>179</v>
+        <v>265</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C87" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>183</v>
-      </c>
-      <c r="B88" t="s">
-        <v>184</v>
-      </c>
-      <c r="C88" t="s">
-        <v>185</v>
+        <v>266</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>242</v>
+        <v>84</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>275</v>
+        <v>161</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>243</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>162</v>
+      </c>
+      <c r="B90" t="s">
+        <v>261</v>
+      </c>
+      <c r="C90" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>263</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>265</v>
+        <v>176</v>
+      </c>
+      <c r="B91" t="s">
+        <v>177</v>
+      </c>
+      <c r="C91" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>269</v>
+        <v>179</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>271</v>
+        <v>180</v>
+      </c>
+      <c r="C92" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
+      <c r="A93" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" t="s">
+        <v>184</v>
+      </c>
+      <c r="C93" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>290</v>
+        <v>241</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>301</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>303</v>
+        <v>242</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>304</v>
+        <v>262</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>306</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>307</v>
+        <v>268</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>308</v>
+        <v>269</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>309</v>
+        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -2955,13 +3055,13 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -2973,6 +3073,54 @@
       </c>
       <c r="C100" s="1" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>301</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>304</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>290</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>295</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pass tests with Orchestrator 2019.10
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313EBB62-B5AB-427E-BACB-C083C3EC7B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA149C1-2D83-41DA-9C65-C170C473CDA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,12 +1103,6 @@
     <t>Invalid value.</t>
   </si>
   <si>
-    <t>https://win-9d2vvsqpta7/</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>ユーザー名の編集に新しいパスワードが必要です。</t>
   </si>
   <si>
@@ -1158,6 +1152,12 @@
   </si>
   <si>
     <t>CreateCredentialAssetIDColumn</t>
+  </si>
+  <si>
+    <t>https://platform.uipath.com</t>
+  </si>
+  <si>
+    <t>MateusTenant</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1541,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1567,7 +1567,7 @@
         <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>355</v>
+        <v>372</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>308</v>
@@ -1578,20 +1578,17 @@
         <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>356</v>
+        <v>373</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>309</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7B9ACE39-67E0-4AAE-B10F-7C3353C799CD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1800,7 +1797,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -1811,13 +1808,13 @@
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B19" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1833,13 +1830,13 @@
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2360,24 +2357,24 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>361</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>362</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -2643,24 +2640,24 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>358</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Adjust formatting of forms
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FCF815-993A-4BD1-AA63-BAB0470CB6D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14E75CC-7AA4-4B96-8370-02BC19127264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -1597,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,7 +1646,7 @@
         <v>256</v>
       </c>
       <c r="B4">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>307</v>
@@ -1657,7 +1657,7 @@
         <v>257</v>
       </c>
       <c r="B5">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>308</v>
@@ -2050,7 +2050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Extract HTTP requests and wrap them with error handling
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14E75CC-7AA4-4B96-8370-02BC19127264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7EFDF1-DF3A-4064-BD97-5CDC0CCC7ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="384">
   <si>
     <t>Name</t>
   </si>
@@ -1158,6 +1158,36 @@
   </si>
   <si>
     <t>FormOULabel</t>
+  </si>
+  <si>
+    <t>UnsupportedHTTPMethod</t>
+  </si>
+  <si>
+    <t>Unsupported HTTP method specified.</t>
+  </si>
+  <si>
+    <t>指定されたHTTPメソッドが対応できません。</t>
+  </si>
+  <si>
+    <t>MakeHTTPRequestNumberOfRetries</t>
+  </si>
+  <si>
+    <t>MakeHTTPRequestRetryInterval</t>
+  </si>
+  <si>
+    <t>Maximum number of times a HTTP request should be retried in case of failure due to connectivity issues.</t>
+  </si>
+  <si>
+    <t>ConnectivityIssuesFailure</t>
+  </si>
+  <si>
+    <t>HTTP Request failed due to connectivity issues.</t>
+  </si>
+  <si>
+    <t>ネットワークの問題のため、リクエストが失敗しました。</t>
+  </si>
+  <si>
+    <t>Interval (in milliseconds) between retries of making a HTTP request.</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1282,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C39" totalsRowShown="0">
-  <autoFilter ref="A1:C39" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C41" totalsRowShown="0">
+  <autoFilter ref="A1:C41" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -1264,8 +1294,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C105" totalsRowShown="0">
-  <autoFilter ref="A1:C105" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C107" totalsRowShown="0">
+  <autoFilter ref="A1:C107" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1595,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1663,141 +1693,141 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" t="s">
-        <v>242</v>
+        <v>377</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>310</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B7" t="s">
-        <v>243</v>
+        <v>378</v>
+      </c>
+      <c r="B7">
+        <v>5000</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>247</v>
+        <v>201</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B10" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>229</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>245</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>83</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>368</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -1808,232 +1838,254 @@
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>364</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>365</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>368</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>366</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>331</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>67</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>322</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" t="s">
-        <v>239</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>239</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
         <v>66</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>181</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>170</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>171</v>
-      </c>
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>338</v>
+        <v>171</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>341</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>338</v>
+      </c>
+      <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>291</v>
-      </c>
-      <c r="B37" t="s">
-        <v>59</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>341</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>291</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>290</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>239</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>304</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>335</v>
       </c>
     </row>
@@ -2048,10 +2100,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2469,654 +2521,676 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>374</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>44</v>
+        <v>375</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>45</v>
+        <v>376</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>380</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>106</v>
+        <v>381</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="A49" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>87</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>349</v>
+        <v>113</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>351</v>
+        <v>114</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>350</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>354</v>
+        <v>119</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>353</v>
+        <v>124</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>352</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="A58" t="s">
+        <v>354</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>355</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>137</v>
+        <v>356</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>138</v>
+        <v>357</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>139</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>268</v>
+        <v>192</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>269</v>
+        <v>193</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>270</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>281</v>
+        <v>195</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>282</v>
+        <v>196</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>283</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="A68" t="s">
+        <v>281</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>275</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>187</v>
+        <v>276</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>75</v>
+        <v>277</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>79</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="A77" t="s">
+        <v>166</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>91</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>49</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>272</v>
+        <v>49</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>274</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>154</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>272</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>88</v>
+        <v>273</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>110</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>112</v>
+        <v>274</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>262</v>
+        <v>116</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>263</v>
+        <v>117</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>264</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>262</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>160</v>
+        <v>263</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>161</v>
-      </c>
-      <c r="B90" t="s">
-        <v>258</v>
-      </c>
-      <c r="C90" t="s">
-        <v>162</v>
+        <v>264</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>175</v>
-      </c>
-      <c r="B91" t="s">
-        <v>176</v>
-      </c>
-      <c r="C91" t="s">
-        <v>177</v>
+        <v>84</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>178</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
+      </c>
+      <c r="B92" t="s">
+        <v>258</v>
       </c>
       <c r="C92" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B93" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C93" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>240</v>
+        <v>178</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>241</v>
+        <v>179</v>
+      </c>
+      <c r="C94" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>182</v>
+      </c>
+      <c r="B95" t="s">
+        <v>183</v>
+      </c>
+      <c r="C95" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>240</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>259</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>265</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>295</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>297</v>
-      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
+      <c r="A103" t="s">
+        <v>298</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>301</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>287</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>292</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>294</v>
       </c>
     </row>

</xml_diff>